<commit_message>
deleted Response.java. updated last modified handling
</commit_message>
<xml_diff>
--- a/Documents/회사평가표_AA조.xlsx
+++ b/Documents/회사평가표_AA조.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seongmoon/PITT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3627140-35F3-864E-97D8-B54CC9D1CC3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE00CFA-4CEC-E946-9951-212BFA629E1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,10 +93,6 @@
     <t>Web Browser가 해석할 수 있는 http response를 구성</t>
   </si>
   <si>
-    <t>해석을 마친 http request에 대해서 올바른 http response의 형태가 무엇인지 이해하고 예외 상황들을 고려하여 Web Browser가 해석할 수 있는 응답을 내보낼 수 있다.
-200 OK, 302 Not modified, 400 Bad request, 404 Not found, 500 Service unavailable 의 다섯가지 응답 형태를 올바로 구현했다.</t>
-  </si>
-  <si>
     <t>구현 항목당 3점
 (총 15점)</t>
   </si>
@@ -159,6 +155,11 @@
   <si>
     <t>비정상적인 client가 event loop에 미치는 영향에 대해서 이해하고 이것으로 인해 전체의 performance에 영향이 가지 않도록 하기 위한 몇가지 기법들에 대해 이해하고 구현한다.
 (read buffer 확장, request timeout)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>해석을 마친 http request에 대해서 올바른 http response의 형태가 무엇인지 이해하고 예외 상황들을 고려하여 Web Browser가 해석할 수 있는 응답을 내보낼 수 있다.
+200 OK, 304 Not modified, 400 Bad request, 404 Not found, 500 Service unavailable 의 다섯가지 응답 형태를 올바로 구현했다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -317,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,31 +353,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -386,17 +362,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -719,8 +717,8 @@
   </sheetPr>
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -770,22 +768,22 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>15</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="25" t="s">
-        <v>41</v>
+      <c r="E2" s="16"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -808,18 +806,18 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
         <v>7</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25" t="s">
-        <v>40</v>
+      <c r="E3" s="17"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -842,15 +840,15 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="24" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -874,17 +872,17 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>15</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -908,15 +906,15 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -940,15 +938,15 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="8">
         <v>5</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -972,17 +970,17 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="54" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>42</v>
+      <c r="C8" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1006,15 +1004,15 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="27" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1038,10 +1036,10 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="67" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1050,7 +1048,7 @@
       <c r="D10" s="2">
         <v>15</v>
       </c>
-      <c r="E10" s="19"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1074,15 +1072,15 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A11" s="21"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="23" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="4">
         <v>12</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1106,15 +1104,15 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1138,17 +1136,17 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="19"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1172,11 +1170,11 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="14"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1200,19 +1198,19 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="55" customHeight="1">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="29" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D15" s="2">
         <v>20</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1236,15 +1234,15 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="55" customHeight="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="6" t="s">
-        <v>28</v>
+      <c r="A16" s="20"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D16" s="4">
         <v>12</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1268,15 +1266,15 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="27" t="s">
-        <v>29</v>
+      <c r="A17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="8">
         <v>4</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1300,19 +1298,19 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="C18" s="29" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="2">
         <v>5</v>
       </c>
-      <c r="E18" s="19"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1336,15 +1334,15 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="30" t="s">
-        <v>33</v>
+      <c r="A19" s="21"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="8">
         <v>3</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1368,19 +1366,19 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="C20" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1404,15 +1402,15 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1436,15 +1434,15 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="8">
         <v>1</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1469,10 +1467,10 @@
     </row>
     <row r="23" spans="1:26" ht="14">
       <c r="A23" s="5"/>
-      <c r="B23" s="25"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="11">
         <f>SUM(E1:E22)</f>
@@ -29194,6 +29192,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E7"/>
@@ -29210,13 +29215,6 @@
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
added node js server. credit to KYS
</commit_message>
<xml_diff>
--- a/Documents/회사평가표_AA조.xlsx
+++ b/Documents/회사평가표_AA조.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seongmoon/PITT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE00CFA-4CEC-E946-9951-212BFA629E1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765F5E9A-43F7-C744-ADA6-77119FF2A957}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -365,6 +365,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -379,24 +390,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -718,7 +721,7 @@
   <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -768,19 +771,19 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>15</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="12"/>
       <c r="G2" s="14" t="s">
         <v>40</v>
@@ -806,15 +809,15 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
         <v>7</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="13"/>
       <c r="G3" s="14" t="s">
         <v>39</v>
@@ -840,15 +843,15 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -872,17 +875,17 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>15</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -906,15 +909,15 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -938,15 +941,15 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="8">
         <v>5</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -970,17 +973,17 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="54" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1004,15 +1007,15 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1036,10 +1039,10 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="67" customHeight="1">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1048,7 +1051,7 @@
       <c r="D10" s="2">
         <v>15</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1072,15 +1075,15 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="4">
         <v>12</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1104,15 +1107,15 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1136,17 +1139,17 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1170,11 +1173,11 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="18"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1198,19 +1201,19 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="55" customHeight="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2">
         <v>20</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1234,15 +1237,15 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="55" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4">
         <v>12</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1266,15 +1269,15 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="8">
         <v>4</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1298,19 +1301,19 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="2">
         <v>5</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1334,15 +1337,15 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="15" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="8">
         <v>3</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1366,10 +1369,10 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1378,7 +1381,7 @@
       <c r="D20" s="4">
         <v>5</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1402,15 +1405,15 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1434,15 +1437,15 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="8">
         <v>1</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -29192,13 +29195,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E7"/>
@@ -29215,6 +29211,13 @@
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>